<commit_message>
Add: some functions to save the results and display the results better
</commit_message>
<xml_diff>
--- a/data/WHOdata.xlsx
+++ b/data/WHOdata.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>